<commit_message>
Loocal phone for tests
</commit_message>
<xml_diff>
--- a/recipients_conge.xlsx
+++ b/recipients_conge.xlsx
@@ -22,7 +22,7 @@
     <t>Telephone</t>
   </si>
   <si>
-    <t>+221 77 857 75 00</t>
+    <t>+224 628 11 11 86</t>
   </si>
 </sst>
 </file>
@@ -46,7 +46,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -60,6 +60,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -82,29 +89,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -432,7 +432,7 @@
     <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2">
         <v>0</v>
       </c>

</xml_diff>